<commit_message>
[Improve] Add opcode STOREsecaccu
</commit_message>
<xml_diff>
--- a/Vivado_nanoProcesseur/260_FPGA_IO_xdc_220908a.xlsx
+++ b/Vivado_nanoProcesseur/260_FPGA_IO_xdc_220908a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Hearc/Di Applied/Vivado_nanoProcesseur/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/Vivado_nanoProcesseur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{FF21D432-8AF7-42D6-888B-FD91FF852052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE771C25-222D-46E9-97B4-9E1ECDC507AD}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{FF21D432-8AF7-42D6-888B-FD91FF852052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B1CFB2C-823B-4F12-AA7D-B8230F9D6E74}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-3255" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XDC_Sysnum" sheetId="6" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="216">
   <si>
     <t>Pin</t>
   </si>
@@ -700,9 +700,6 @@
     <t>reset_i</t>
   </si>
   <si>
-    <t>signal</t>
-  </si>
-  <si>
     <t>port_a_i</t>
   </si>
   <si>
@@ -719,6 +716,12 @@
   </si>
   <si>
     <t>PCounter_o</t>
+  </si>
+  <si>
+    <t>port_c_o</t>
+  </si>
+  <si>
+    <t>port_c_4i</t>
   </si>
 </sst>
 </file>
@@ -1292,6 +1295,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="xc7a35tfgg484pkg" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -1569,7 +1576,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,7 +1705,7 @@
         <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -1736,7 +1743,7 @@
         <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1774,7 +1781,7 @@
         <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -1812,7 +1819,7 @@
         <v>140</v>
       </c>
       <c r="D7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
@@ -1850,7 +1857,7 @@
         <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
@@ -1888,7 +1895,7 @@
         <v>141</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
@@ -1926,7 +1933,7 @@
         <v>136</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E10" s="1">
         <v>6</v>
@@ -1964,7 +1971,7 @@
         <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E11" s="1">
         <v>7</v>
@@ -2002,7 +2009,7 @@
         <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -2040,7 +2047,7 @@
         <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -2078,7 +2085,7 @@
         <v>145</v>
       </c>
       <c r="D14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -2116,7 +2123,7 @@
         <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -2154,7 +2161,7 @@
         <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E16" s="1">
         <v>4</v>
@@ -2192,7 +2199,7 @@
         <v>146</v>
       </c>
       <c r="D17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E17" s="1">
         <v>5</v>
@@ -2230,7 +2237,7 @@
         <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E18" s="1">
         <v>6</v>
@@ -2268,7 +2275,7 @@
         <v>147</v>
       </c>
       <c r="D19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E19" s="1">
         <v>7</v>
@@ -2306,7 +2313,7 @@
         <v>173</v>
       </c>
       <c r="D20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -2344,7 +2351,7 @@
         <v>175</v>
       </c>
       <c r="D21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -2382,7 +2389,7 @@
         <v>176</v>
       </c>
       <c r="D22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E22" s="1">
         <v>2</v>
@@ -2420,7 +2427,7 @@
         <v>177</v>
       </c>
       <c r="D23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -2458,7 +2465,7 @@
         <v>178</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E24" s="1">
         <v>4</v>
@@ -2496,7 +2503,7 @@
         <v>179</v>
       </c>
       <c r="D25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E25" s="1">
         <v>5</v>
@@ -2534,7 +2541,7 @@
         <v>180</v>
       </c>
       <c r="D26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E26" s="1">
         <v>6</v>
@@ -2572,7 +2579,7 @@
         <v>181</v>
       </c>
       <c r="D27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E27" s="1">
         <v>7</v>
@@ -2680,13 +2687,13 @@
         <v>174</v>
       </c>
       <c r="D30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G30" s="15" t="str">
         <f>IF(D30="","",J30&amp;REPT(" ",MAX(I:I)-I30)&amp;" "&amp;K30)</f>
@@ -2717,13 +2724,13 @@
         <v>184</v>
       </c>
       <c r="D31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G31" s="15" t="str">
         <f>IF(D31="","",J31&amp;REPT(" ",MAX(I:I)-I31)&amp;" "&amp;K31)</f>
@@ -2754,13 +2761,13 @@
         <v>185</v>
       </c>
       <c r="D32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E32" s="1">
         <v>2</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G32" s="15" t="str">
         <f t="shared" si="5"/>
@@ -2791,7 +2798,7 @@
         <v>186</v>
       </c>
       <c r="D33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E33" s="1">
         <v>3</v>
@@ -2829,7 +2836,7 @@
         <v>187</v>
       </c>
       <c r="D34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E34" s="1">
         <v>4</v>
@@ -2867,7 +2874,7 @@
         <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E35" s="1">
         <v>5</v>
@@ -2905,7 +2912,7 @@
         <v>189</v>
       </c>
       <c r="D36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E36" s="1">
         <v>6</v>
@@ -2943,7 +2950,7 @@
         <v>190</v>
       </c>
       <c r="D37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E37" s="1">
         <v>7</v>
@@ -3191,7 +3198,7 @@
         <v>160</v>
       </c>
       <c r="D44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -3229,7 +3236,7 @@
         <v>161</v>
       </c>
       <c r="D45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -3267,7 +3274,7 @@
         <v>162</v>
       </c>
       <c r="D46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E46" s="1">
         <v>2</v>
@@ -3305,7 +3312,7 @@
         <v>163</v>
       </c>
       <c r="D47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E47" s="1">
         <v>3</v>
@@ -3343,7 +3350,7 @@
         <v>164</v>
       </c>
       <c r="D48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E48" s="1">
         <v>4</v>
@@ -3381,7 +3388,7 @@
         <v>165</v>
       </c>
       <c r="D49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -3419,7 +3426,7 @@
         <v>166</v>
       </c>
       <c r="D50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E50" s="1">
         <v>6</v>
@@ -3457,7 +3464,7 @@
         <v>167</v>
       </c>
       <c r="D51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E51" s="1">
         <v>7</v>
@@ -3529,25 +3536,32 @@
       <c r="C53" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>208</v>
+      <c r="D53" t="s">
+        <v>215</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>bus</v>
       </c>
       <c r="G53" s="15" t="str">
         <f>IF(D53="","",J53&amp;REPT(" ",MAX(I:I)-I53)&amp;" "&amp;K53)</f>
-        <v/>
+        <v>set_property PACKAGE_PIN U21   [get_ports port_c_4i[0]];  set_property IOSTANDARD LVCMOS33 [get_ports port_c_4i[0]]</v>
       </c>
       <c r="H53" s="8"/>
       <c r="I53" s="13">
         <f t="shared" si="13"/>
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="J53" s="14" t="str">
         <f>"set_property PACKAGE_PIN "&amp;A53&amp;REPT(" ",5-LEN(A53))&amp;" [get_ports "&amp;D53&amp;IF(ISBLANK(E53),"","["&amp;E53&amp;"]")&amp;"];"</f>
-        <v>set_property PACKAGE_PIN U21   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN U21   [get_ports port_c_4i[0]];</v>
       </c>
       <c r="K53" s="14" t="str">
         <f>"set_property IOSTANDARD LVCMOS33 [get_ports "&amp;D53&amp;IF(ISBLANK(E53),"","["&amp;E53&amp;"]")&amp;"]"</f>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_4i[0]]</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3560,26 +3574,32 @@
       <c r="C54" s="11" t="s">
         <v>157</v>
       </c>
+      <c r="D54" t="s">
+        <v>215</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
       <c r="F54" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G54" s="15" t="str">
         <f>IF(D54="","",J54&amp;REPT(" ",MAX(I:I)-I54)&amp;" "&amp;K54)</f>
-        <v/>
+        <v>set_property PACKAGE_PIN V20   [get_ports port_c_4i[1]];  set_property IOSTANDARD LVCMOS33 [get_ports port_c_4i[1]]</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="13">
         <f t="shared" si="13"/>
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="J54" s="14" t="str">
         <f t="shared" ref="J54:J57" si="14">"set_property PACKAGE_PIN "&amp;A54&amp;REPT(" ",5-LEN(A54))&amp;" [get_ports "&amp;D54&amp;IF(ISBLANK(E54),"","["&amp;E54&amp;"]")&amp;"];"</f>
-        <v>set_property PACKAGE_PIN V20   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN V20   [get_ports port_c_4i[1]];</v>
       </c>
       <c r="K54" s="14" t="str">
         <f t="shared" ref="K54:K57" si="15">"set_property IOSTANDARD LVCMOS33 [get_ports "&amp;D54&amp;IF(ISBLANK(E54),"","["&amp;E54&amp;"]")&amp;"]"</f>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_4i[1]]</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3592,26 +3612,32 @@
       <c r="C55" s="11" t="s">
         <v>158</v>
       </c>
+      <c r="D55" t="s">
+        <v>215</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2</v>
+      </c>
       <c r="F55" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G55" s="15" t="str">
         <f>IF(D55="","",J55&amp;REPT(" ",MAX(I:I)-I55)&amp;" "&amp;K55)</f>
-        <v/>
+        <v>set_property PACKAGE_PIN W20   [get_ports port_c_4i[2]];  set_property IOSTANDARD LVCMOS33 [get_ports port_c_4i[2]]</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="13">
         <f t="shared" si="13"/>
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="J55" s="14" t="str">
         <f t="shared" si="14"/>
-        <v>set_property PACKAGE_PIN W20   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN W20   [get_ports port_c_4i[2]];</v>
       </c>
       <c r="K55" s="14" t="str">
         <f t="shared" si="15"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_4i[2]]</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3624,26 +3650,32 @@
       <c r="C56" s="11" t="s">
         <v>159</v>
       </c>
+      <c r="D56" t="s">
+        <v>215</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3</v>
+      </c>
       <c r="F56" s="1" t="str">
         <f>IF(ISNUMBER(E56),"bus","signal")</f>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G56" s="15" t="str">
         <f>IF(D56="","",J56&amp;REPT(" ",MAX(I:I)-I56)&amp;" "&amp;K56)</f>
-        <v/>
+        <v>set_property PACKAGE_PIN U20   [get_ports port_c_4i[3]];  set_property IOSTANDARD LVCMOS33 [get_ports port_c_4i[3]]</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="13">
         <f t="shared" si="13"/>
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="J56" s="14" t="str">
         <f t="shared" si="14"/>
-        <v>set_property PACKAGE_PIN U20   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN U20   [get_ports port_c_4i[3]];</v>
       </c>
       <c r="K56" s="14" t="str">
         <f t="shared" si="15"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_4i[3]]</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3688,26 +3720,32 @@
       <c r="C58" s="12" t="s">
         <v>148</v>
       </c>
+      <c r="D58" t="s">
+        <v>214</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
       <c r="F58" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G58" s="15" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>set_property PACKAGE_PIN A18   [get_ports port_c_o[0]];   set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[0]]</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="13">
         <f t="shared" ref="I58:I65" si="16">LEN(J58)</f>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J58" s="14" t="str">
         <f t="shared" ref="J58:J65" si="17">"set_property PACKAGE_PIN "&amp;A58&amp;REPT(" ",5-LEN(A58))&amp;" [get_ports "&amp;D58&amp;IF(ISBLANK(E58),"","["&amp;E58&amp;"]")&amp;"];"</f>
-        <v>set_property PACKAGE_PIN A18   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN A18   [get_ports port_c_o[0]];</v>
       </c>
       <c r="K58" s="14" t="str">
         <f t="shared" ref="K58:K65" si="18">"set_property IOSTANDARD LVCMOS33 [get_ports "&amp;D58&amp;IF(ISBLANK(E58),"","["&amp;E58&amp;"]")&amp;"]"</f>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[0]]</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3720,26 +3758,32 @@
       <c r="C59" s="12" t="s">
         <v>149</v>
       </c>
+      <c r="D59" t="s">
+        <v>214</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
       <c r="F59" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G59" s="15" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>set_property PACKAGE_PIN B20   [get_ports port_c_o[1]];   set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[1]]</v>
       </c>
       <c r="H59" s="8"/>
       <c r="I59" s="13">
         <f t="shared" si="16"/>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J59" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>set_property PACKAGE_PIN B20   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN B20   [get_ports port_c_o[1]];</v>
       </c>
       <c r="K59" s="14" t="str">
         <f t="shared" si="18"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[1]]</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -3752,26 +3796,32 @@
       <c r="C60" s="12" t="s">
         <v>150</v>
       </c>
+      <c r="D60" t="s">
+        <v>214</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2</v>
+      </c>
       <c r="F60" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G60" s="15" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>set_property PACKAGE_PIN A20   [get_ports port_c_o[2]];   set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[2]]</v>
       </c>
       <c r="H60" s="8"/>
       <c r="I60" s="13">
         <f t="shared" si="16"/>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J60" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>set_property PACKAGE_PIN A20   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN A20   [get_ports port_c_o[2]];</v>
       </c>
       <c r="K60" s="14" t="str">
         <f t="shared" si="18"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[2]]</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -3784,26 +3834,32 @@
       <c r="C61" s="12" t="s">
         <v>151</v>
       </c>
+      <c r="D61" t="s">
+        <v>214</v>
+      </c>
+      <c r="E61" s="1">
+        <v>3</v>
+      </c>
       <c r="F61" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G61" s="15" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>set_property PACKAGE_PIN B21   [get_ports port_c_o[3]];   set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[3]]</v>
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="13">
         <f t="shared" si="16"/>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J61" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>set_property PACKAGE_PIN B21   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN B21   [get_ports port_c_o[3]];</v>
       </c>
       <c r="K61" s="14" t="str">
         <f t="shared" si="18"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[3]]</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3816,26 +3872,32 @@
       <c r="C62" s="12" t="s">
         <v>152</v>
       </c>
+      <c r="D62" t="s">
+        <v>214</v>
+      </c>
+      <c r="E62" s="1">
+        <v>4</v>
+      </c>
       <c r="F62" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G62" s="15" t="str">
         <f>IF(D62="","",J62&amp;REPT(" ",MAX(I:I)-I62)&amp;" "&amp;K62)</f>
-        <v/>
+        <v>set_property PACKAGE_PIN B16   [get_ports port_c_o[4]];   set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[4]]</v>
       </c>
       <c r="H62" s="8"/>
       <c r="I62" s="13">
         <f t="shared" si="16"/>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J62" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>set_property PACKAGE_PIN B16   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN B16   [get_ports port_c_o[4]];</v>
       </c>
       <c r="K62" s="14" t="str">
         <f t="shared" si="18"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[4]]</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -3848,26 +3910,32 @@
       <c r="C63" s="12" t="s">
         <v>153</v>
       </c>
+      <c r="D63" t="s">
+        <v>214</v>
+      </c>
+      <c r="E63" s="1">
+        <v>5</v>
+      </c>
       <c r="F63" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G63" s="15" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>set_property PACKAGE_PIN B18   [get_ports port_c_o[5]];   set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[5]]</v>
       </c>
       <c r="H63" s="8"/>
       <c r="I63" s="13">
         <f t="shared" si="16"/>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J63" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>set_property PACKAGE_PIN B18   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN B18   [get_ports port_c_o[5]];</v>
       </c>
       <c r="K63" s="14" t="str">
         <f t="shared" si="18"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[5]]</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -3880,26 +3948,32 @@
       <c r="C64" s="12" t="s">
         <v>154</v>
       </c>
+      <c r="D64" t="s">
+        <v>214</v>
+      </c>
+      <c r="E64" s="1">
+        <v>6</v>
+      </c>
       <c r="F64" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G64" s="15" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>set_property PACKAGE_PIN A19   [get_ports port_c_o[6]];   set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[6]]</v>
       </c>
       <c r="H64" s="8"/>
       <c r="I64" s="13">
         <f t="shared" si="16"/>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J64" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>set_property PACKAGE_PIN A19   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN A19   [get_ports port_c_o[6]];</v>
       </c>
       <c r="K64" s="14" t="str">
         <f t="shared" si="18"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[6]]</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -3912,26 +3986,32 @@
       <c r="C65" s="12" t="s">
         <v>155</v>
       </c>
+      <c r="D65" t="s">
+        <v>214</v>
+      </c>
+      <c r="E65" s="1">
+        <v>7</v>
+      </c>
       <c r="F65" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>signal</v>
+        <v>bus</v>
       </c>
       <c r="G65" s="15" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>set_property PACKAGE_PIN A21   [get_ports port_c_o[7]];   set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[7]]</v>
       </c>
       <c r="H65" s="8"/>
       <c r="I65" s="13">
         <f t="shared" si="16"/>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J65" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>set_property PACKAGE_PIN A21   [get_ports ];</v>
+        <v>set_property PACKAGE_PIN A21   [get_ports port_c_o[7]];</v>
       </c>
       <c r="K65" s="14" t="str">
         <f t="shared" si="18"/>
-        <v>set_property IOSTANDARD LVCMOS33 [get_ports ]</v>
+        <v>set_property IOSTANDARD LVCMOS33 [get_ports port_c_o[7]]</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>